<commit_message>
Update mzML convert generator.xlsx
</commit_message>
<xml_diff>
--- a/demo data/HDX-MS raw data/utilities/mzML convert generator.xlsx
+++ b/demo data/HDX-MS raw data/utilities/mzML convert generator.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubordeauxfr-my.sharepoint.com/personal/eric_largy_u-bordeaux_fr/Documents/Git/OligoR_reboot/demo data/HDX-MS raw data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\users\RG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="8_{E099697F-4EDF-4311-9AEA-37C88FF1C264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC4E1B2E-D4E8-4A90-99BB-FA64B52F6F57}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="37710" windowHeight="21840" activeTab="3" xr2:uid="{832DC8D8-CB75-4467-96A4-FC9121A9F707}"/>
+    <workbookView xWindow="39764" yWindow="670" windowWidth="25478" windowHeight="15612" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="23TAG" sheetId="2" r:id="rId1"/>
     <sheet name="23TAG-PhenDC3" sheetId="1" r:id="rId2"/>
     <sheet name="T30177-TT" sheetId="3" r:id="rId3"/>
     <sheet name="VEGF" sheetId="4" r:id="rId4"/>
+    <sheet name="5YEY" sheetId="5" r:id="rId5"/>
+    <sheet name="5YEY-zone1" sheetId="6" r:id="rId6"/>
+    <sheet name="2KPR" sheetId="7" r:id="rId7"/>
+    <sheet name="23TAGIMS" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="46">
   <si>
     <t>tube</t>
   </si>
@@ -106,12 +109,81 @@
   <si>
     <t>REF</t>
   </si>
+  <si>
+    <t>T0-1</t>
+  </si>
+  <si>
+    <t>T0-2</t>
+  </si>
+  <si>
+    <t>T1-1</t>
+  </si>
+  <si>
+    <t>T1-2</t>
+  </si>
+  <si>
+    <t>T2-1</t>
+  </si>
+  <si>
+    <t>T2-2</t>
+  </si>
+  <si>
+    <t>T3-1</t>
+  </si>
+  <si>
+    <t>T3-2</t>
+  </si>
+  <si>
+    <t>T3-3</t>
+  </si>
+  <si>
+    <t>T4-1</t>
+  </si>
+  <si>
+    <t>T4-2</t>
+  </si>
+  <si>
+    <t>T4-3</t>
+  </si>
+  <si>
+    <t>T5-1</t>
+  </si>
+  <si>
+    <t>T5-2</t>
+  </si>
+  <si>
+    <t>T5-3</t>
+  </si>
+  <si>
+    <t>T6-1</t>
+  </si>
+  <si>
+    <t>T6-2</t>
+  </si>
+  <si>
+    <t>T6-3</t>
+  </si>
+  <si>
+    <t>T7-1</t>
+  </si>
+  <si>
+    <t>T7-2</t>
+  </si>
+  <si>
+    <t>T7-3</t>
+  </si>
+  <si>
+    <t>RTHDX</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +203,13 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -154,15 +233,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="30">
     <dxf>
       <font>
         <b/>
@@ -177,7 +257,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -195,7 +274,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -221,7 +299,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -239,7 +316,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -265,7 +341,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -283,7 +358,174 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -306,7 +548,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -324,7 +565,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -347,21 +587,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{82A29707-108A-4827-A26A-6ABB22E4E27F}" name="Table13" displayName="Table13" ref="F6:M28" totalsRowShown="0">
-  <autoFilter ref="F6:M28" xr:uid="{82A29707-108A-4827-A26A-6ABB22E4E27F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="F6:M28" totalsRowShown="0">
+  <autoFilter ref="F6:M28"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{7C8F1A9C-3243-4FC5-A0A0-0F8D7ACEE8B0}" name="tube"/>
-    <tableColumn id="2" xr3:uid="{2DD4AE8C-0ECA-44D6-A89C-10CD443D1A22}" name="start.min"/>
-    <tableColumn id="3" xr3:uid="{E41327CC-BC7C-4292-9063-7F51666368F7}" name="end.min">
+    <tableColumn id="1" name="tube"/>
+    <tableColumn id="2" name="start.min"/>
+    <tableColumn id="3" name="end.min">
       <calculatedColumnFormula>G7+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0B7A98A3-E4CD-4F25-86F1-C773704BAF27}" name="start.mz"/>
-    <tableColumn id="8" xr3:uid="{862BD483-61A0-4468-B386-0E30C9CCE61F}" name="end.mz"/>
-    <tableColumn id="6" xr3:uid="{1DBC6E8D-8193-4A4D-9E00-2FFF8E3418F6}" name="pt" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{BDD30EE1-32BE-4E72-B432-776CB76893AC}" name="start.s" dataDxfId="9">
+    <tableColumn id="7" name="start.mz"/>
+    <tableColumn id="8" name="end.mz"/>
+    <tableColumn id="6" name="pt" dataDxfId="29"/>
+    <tableColumn id="4" name="start.s" dataDxfId="28">
       <calculatedColumnFormula>G7*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{765C5F9A-C3EE-4AB4-B02C-DDCB045ECD83}" name="end.s" dataDxfId="8">
+    <tableColumn id="5" name="end.s" dataDxfId="27">
       <calculatedColumnFormula>H7*60</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -370,21 +610,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{537B99D1-DC23-493A-927F-9D8D5889E9D2}" name="Table1" displayName="Table1" ref="H5:O27" totalsRowShown="0">
-  <autoFilter ref="H5:O27" xr:uid="{537B99D1-DC23-493A-927F-9D8D5889E9D2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="H5:O27" totalsRowShown="0">
+  <autoFilter ref="H5:O27"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{AB2AFD76-86ED-4122-856C-A5DA9D48ADE3}" name="tube"/>
-    <tableColumn id="2" xr3:uid="{C584EA24-5442-408A-A884-030B9D2BCACF}" name="start.min"/>
-    <tableColumn id="3" xr3:uid="{7088ED6B-2127-44EA-B6F2-521B3177FF7C}" name="end.min">
+    <tableColumn id="1" name="tube"/>
+    <tableColumn id="2" name="start.min"/>
+    <tableColumn id="3" name="end.min">
       <calculatedColumnFormula>I6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BA7CC746-A465-4A7D-8A3F-0061FD52C8BD}" name="start.mz"/>
-    <tableColumn id="8" xr3:uid="{F3393A89-97F2-4B7E-A054-ACA25F9187DD}" name="end.mz"/>
-    <tableColumn id="6" xr3:uid="{F8E6BCDC-E128-4319-83CB-9254D864C73A}" name="pt" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{631509AD-9B5D-4D10-82C8-79665AAC8E3D}" name="start.s" dataDxfId="12">
+    <tableColumn id="7" name="start.mz"/>
+    <tableColumn id="8" name="end.mz"/>
+    <tableColumn id="6" name="pt" dataDxfId="26"/>
+    <tableColumn id="4" name="start.s" dataDxfId="25">
       <calculatedColumnFormula>I6*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5B4E67B-26A5-44BD-9717-0ECB44E6A769}" name="end.s" dataDxfId="11">
+    <tableColumn id="5" name="end.s" dataDxfId="24">
       <calculatedColumnFormula>J6*60</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -393,21 +633,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CF2EEE27-1C21-4273-AF01-46759B6DC9DF}" name="Table134" displayName="Table134" ref="F6:M27" totalsRowShown="0">
-  <autoFilter ref="F6:M27" xr:uid="{82A29707-108A-4827-A26A-6ABB22E4E27F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="F6:M27" totalsRowShown="0">
+  <autoFilter ref="F6:M27"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{2D716382-00C2-43F6-AE8A-94123DBA7B83}" name="tube" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{57A56B7F-C16C-4DC2-826D-3B7F3D2F02C8}" name="start.min"/>
-    <tableColumn id="3" xr3:uid="{1C08E95C-B92A-4F09-986A-E9827F5D9FD2}" name="end.min">
+    <tableColumn id="1" name="tube" dataDxfId="23"/>
+    <tableColumn id="2" name="start.min"/>
+    <tableColumn id="3" name="end.min">
       <calculatedColumnFormula>G7+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B094506A-2271-473F-A4D3-2500051F5B16}" name="start.mz"/>
-    <tableColumn id="8" xr3:uid="{7A217C86-9A8D-4F07-BD82-A210756B4F12}" name="end.mz"/>
-    <tableColumn id="6" xr3:uid="{A21BB671-1A4E-4501-A830-EA9AC0696EB8}" name="pt" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{1BC31107-15D7-4D1A-893E-80885DAC11A2}" name="start.s" dataDxfId="5">
+    <tableColumn id="7" name="start.mz"/>
+    <tableColumn id="8" name="end.mz"/>
+    <tableColumn id="6" name="pt" dataDxfId="22"/>
+    <tableColumn id="4" name="start.s" dataDxfId="21">
       <calculatedColumnFormula>G7*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{77834B75-10E9-4BEF-B346-319DCD321FAA}" name="end.s" dataDxfId="4">
+    <tableColumn id="5" name="end.s" dataDxfId="20">
       <calculatedColumnFormula>H7*60</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -416,21 +656,113 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{08CED98D-A078-4415-AF56-30B1CA2819A4}" name="Table1345" displayName="Table1345" ref="F6:M27" totalsRowShown="0">
-  <autoFilter ref="F6:M27" xr:uid="{82A29707-108A-4827-A26A-6ABB22E4E27F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1345" displayName="Table1345" ref="F6:M27" totalsRowShown="0">
+  <autoFilter ref="F6:M27"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B5D83924-B855-4644-A52F-5FAE3CE55B27}" name="tube" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{2FFAA775-8333-4480-9FFF-5AC309EE3D9E}" name="start.min"/>
-    <tableColumn id="3" xr3:uid="{F7B3CCEF-F45D-41EC-B574-7DC171C4ED74}" name="end.min">
+    <tableColumn id="1" name="tube" dataDxfId="19"/>
+    <tableColumn id="2" name="start.min"/>
+    <tableColumn id="3" name="end.min">
       <calculatedColumnFormula>G7+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{92522D21-7F93-4410-8E48-9C0E75B7400A}" name="start.mz"/>
-    <tableColumn id="8" xr3:uid="{0723D45B-7C65-4293-AA11-273D25BDDB06}" name="end.mz"/>
-    <tableColumn id="6" xr3:uid="{947047F4-31E4-4F27-9E34-FB0878ED0B03}" name="pt" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{F15BDF93-575B-4E91-9B7A-A885D3D96CDA}" name="start.s" dataDxfId="1">
+    <tableColumn id="7" name="start.mz"/>
+    <tableColumn id="8" name="end.mz"/>
+    <tableColumn id="6" name="pt" dataDxfId="18"/>
+    <tableColumn id="4" name="start.s" dataDxfId="17">
       <calculatedColumnFormula>G7*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7B4B767A-5BD6-4655-9480-251A966E159D}" name="end.s" dataDxfId="0">
+    <tableColumn id="5" name="end.s" dataDxfId="16">
+      <calculatedColumnFormula>H7*60</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13456" displayName="Table13456" ref="F6:M27" totalsRowShown="0">
+  <autoFilter ref="F6:M27"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="tube" dataDxfId="15"/>
+    <tableColumn id="2" name="start.min"/>
+    <tableColumn id="3" name="end.min">
+      <calculatedColumnFormula>G7+1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="start.mz"/>
+    <tableColumn id="8" name="end.mz"/>
+    <tableColumn id="6" name="pt" dataDxfId="14"/>
+    <tableColumn id="4" name="start.s" dataDxfId="13">
+      <calculatedColumnFormula>G7*60</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="end.s" dataDxfId="12">
+      <calculatedColumnFormula>H7*60</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table134567" displayName="Table134567" ref="F6:M27" totalsRowShown="0">
+  <autoFilter ref="F6:M27"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="tube" dataDxfId="11"/>
+    <tableColumn id="2" name="start.min"/>
+    <tableColumn id="3" name="end.min">
+      <calculatedColumnFormula>G7+1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="start.mz"/>
+    <tableColumn id="8" name="end.mz"/>
+    <tableColumn id="6" name="pt" dataDxfId="10"/>
+    <tableColumn id="4" name="start.s" dataDxfId="9">
+      <calculatedColumnFormula>G7*60</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="end.s" dataDxfId="8">
+      <calculatedColumnFormula>H7*60</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table1345678" displayName="Table1345678" ref="F6:M29" totalsRowShown="0">
+  <autoFilter ref="F6:M29"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="tube" dataDxfId="7"/>
+    <tableColumn id="2" name="start.min"/>
+    <tableColumn id="3" name="end.min">
+      <calculatedColumnFormula>G7+1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="start.mz"/>
+    <tableColumn id="8" name="end.mz"/>
+    <tableColumn id="6" name="pt" dataDxfId="6"/>
+    <tableColumn id="4" name="start.s" dataDxfId="5">
+      <calculatedColumnFormula>G7*60</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="end.s" dataDxfId="4">
+      <calculatedColumnFormula>H7*60</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table13456789" displayName="Table13456789" ref="F6:M28" totalsRowShown="0">
+  <autoFilter ref="F6:M28"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="tube" dataDxfId="3"/>
+    <tableColumn id="2" name="start.min"/>
+    <tableColumn id="3" name="end.min">
+      <calculatedColumnFormula>G7+1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="start.mz"/>
+    <tableColumn id="8" name="end.mz"/>
+    <tableColumn id="6" name="pt" dataDxfId="2"/>
+    <tableColumn id="4" name="start.s" dataDxfId="1">
+      <calculatedColumnFormula>G7*60</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="end.s" dataDxfId="0">
       <calculatedColumnFormula>H7*60</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -734,14 +1066,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDC913D-3188-40FF-87DE-F74EF846F5B5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F6:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="6" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
@@ -1417,14 +1749,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8ABC03-DD0D-454D-8733-CBF7EFBB0264}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H5:O27"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J6" sqref="J6:O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
@@ -2106,14 +2438,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2DF8B2-7C82-475F-8B80-4F6CF5F515AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F6:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="6" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
@@ -2207,7 +2539,7 @@
         <v>18.5</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H9:H28" si="0">G9+1</f>
+        <f t="shared" ref="H9:H27" si="0">G9+1</f>
         <v>19.5</v>
       </c>
       <c r="I9">
@@ -2220,7 +2552,7 @@
         <v>2</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" ref="L9:M28" si="1">G9*60</f>
+        <f t="shared" ref="L9:M27" si="1">G9*60</f>
         <v>1110</v>
       </c>
       <c r="M9" s="1">
@@ -2770,14 +3102,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22AE4A82-402F-475A-AA90-30D6C1E09D66}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F6:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="6" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
@@ -2871,7 +3203,7 @@
         <v>5</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H9:H28" si="0">G9+1</f>
+        <f t="shared" ref="H9:H27" si="0">G9+1</f>
         <v>6</v>
       </c>
       <c r="I9">
@@ -2884,7 +3216,7 @@
         <v>2</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" ref="L9:M28" si="1">G9*60</f>
+        <f t="shared" ref="L9:M27" si="1">G9*60</f>
         <v>300</v>
       </c>
       <c r="M9" s="1">
@@ -3419,6 +3751,2665 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F6:M27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AG23" sqref="AG23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>1675</v>
+      </c>
+      <c r="J7">
+        <v>1690</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <f>G7*60</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <f>H7*60</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>1675</v>
+      </c>
+      <c r="J8">
+        <v>1690</v>
+      </c>
+      <c r="K8" s="1">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" ref="L8:M26" si="0">G8*60</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>1675</v>
+      </c>
+      <c r="J9">
+        <v>1690</v>
+      </c>
+      <c r="K9" s="1">
+        <v>3</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>1675</v>
+      </c>
+      <c r="J10">
+        <v>1690</v>
+      </c>
+      <c r="K10" s="1">
+        <v>4</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>1675</v>
+      </c>
+      <c r="J11">
+        <v>1690</v>
+      </c>
+      <c r="K11" s="1">
+        <v>5</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>1675</v>
+      </c>
+      <c r="J12">
+        <v>1690</v>
+      </c>
+      <c r="K12" s="1">
+        <v>6</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>1675</v>
+      </c>
+      <c r="J13">
+        <v>1690</v>
+      </c>
+      <c r="K13" s="1">
+        <v>7</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>1675</v>
+      </c>
+      <c r="J14">
+        <v>1690</v>
+      </c>
+      <c r="K14" s="1">
+        <v>8</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>1675</v>
+      </c>
+      <c r="J15">
+        <v>1690</v>
+      </c>
+      <c r="K15" s="1">
+        <v>9</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>1675</v>
+      </c>
+      <c r="J16">
+        <v>1690</v>
+      </c>
+      <c r="K16" s="1">
+        <v>10</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>1675</v>
+      </c>
+      <c r="J17">
+        <v>1690</v>
+      </c>
+      <c r="K17" s="1">
+        <v>11</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>1675</v>
+      </c>
+      <c r="J18">
+        <v>1690</v>
+      </c>
+      <c r="K18" s="1">
+        <v>12</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>1675</v>
+      </c>
+      <c r="J19">
+        <v>1690</v>
+      </c>
+      <c r="K19" s="1">
+        <v>13</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>1675</v>
+      </c>
+      <c r="J20">
+        <v>1690</v>
+      </c>
+      <c r="K20" s="1">
+        <v>14</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>1675</v>
+      </c>
+      <c r="J21">
+        <v>1690</v>
+      </c>
+      <c r="K21" s="1">
+        <v>15</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>1675</v>
+      </c>
+      <c r="J22">
+        <v>1690</v>
+      </c>
+      <c r="K22" s="1">
+        <v>16</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>1675</v>
+      </c>
+      <c r="J23">
+        <v>1690</v>
+      </c>
+      <c r="K23" s="1">
+        <v>17</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="24" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>1675</v>
+      </c>
+      <c r="J24">
+        <v>1690</v>
+      </c>
+      <c r="K24" s="1">
+        <v>18</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>1675</v>
+      </c>
+      <c r="J25">
+        <v>1690</v>
+      </c>
+      <c r="K25" s="1">
+        <v>19</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>1675</v>
+      </c>
+      <c r="J26">
+        <v>1690</v>
+      </c>
+      <c r="K26" s="1">
+        <v>20</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>1675</v>
+      </c>
+      <c r="J27">
+        <v>1690</v>
+      </c>
+      <c r="K27" s="1">
+        <v>21</v>
+      </c>
+      <c r="L27" s="1">
+        <f>G27*60</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="1">
+        <f>H27*60</f>
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F6:M27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>1675</v>
+      </c>
+      <c r="J7">
+        <v>1690</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <f>G7*60</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <f>H7*60</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>1675</v>
+      </c>
+      <c r="J8">
+        <v>1690</v>
+      </c>
+      <c r="K8" s="1">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" ref="L8:M26" si="0">G8*60</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>1675</v>
+      </c>
+      <c r="J9">
+        <v>1690</v>
+      </c>
+      <c r="K9" s="1">
+        <v>3</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>1675</v>
+      </c>
+      <c r="J10">
+        <v>1690</v>
+      </c>
+      <c r="K10" s="1">
+        <v>4</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>1675</v>
+      </c>
+      <c r="J11">
+        <v>1690</v>
+      </c>
+      <c r="K11" s="1">
+        <v>5</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>1675</v>
+      </c>
+      <c r="J12">
+        <v>1690</v>
+      </c>
+      <c r="K12" s="1">
+        <v>6</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>1675</v>
+      </c>
+      <c r="J13">
+        <v>1690</v>
+      </c>
+      <c r="K13" s="1">
+        <v>7</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>1675</v>
+      </c>
+      <c r="J14">
+        <v>1690</v>
+      </c>
+      <c r="K14" s="1">
+        <v>8</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>1675</v>
+      </c>
+      <c r="J15">
+        <v>1690</v>
+      </c>
+      <c r="K15" s="1">
+        <v>9</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>1675</v>
+      </c>
+      <c r="J16">
+        <v>1690</v>
+      </c>
+      <c r="K16" s="1">
+        <v>10</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>1675</v>
+      </c>
+      <c r="J17">
+        <v>1690</v>
+      </c>
+      <c r="K17" s="1">
+        <v>11</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>1675</v>
+      </c>
+      <c r="J18">
+        <v>1690</v>
+      </c>
+      <c r="K18" s="1">
+        <v>12</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>1675</v>
+      </c>
+      <c r="J19">
+        <v>1690</v>
+      </c>
+      <c r="K19" s="1">
+        <v>13</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>1675</v>
+      </c>
+      <c r="J20">
+        <v>1690</v>
+      </c>
+      <c r="K20" s="1">
+        <v>14</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>1675</v>
+      </c>
+      <c r="J21">
+        <v>1690</v>
+      </c>
+      <c r="K21" s="1">
+        <v>15</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>1675</v>
+      </c>
+      <c r="J22">
+        <v>1690</v>
+      </c>
+      <c r="K22" s="1">
+        <v>16</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>1675</v>
+      </c>
+      <c r="J23">
+        <v>1690</v>
+      </c>
+      <c r="K23" s="1">
+        <v>17</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="24" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>1675</v>
+      </c>
+      <c r="J24">
+        <v>1690</v>
+      </c>
+      <c r="K24" s="1">
+        <v>18</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>1675</v>
+      </c>
+      <c r="J25">
+        <v>1690</v>
+      </c>
+      <c r="K25" s="1">
+        <v>19</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>1675</v>
+      </c>
+      <c r="J26">
+        <v>1690</v>
+      </c>
+      <c r="K26" s="1">
+        <v>20</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>1675</v>
+      </c>
+      <c r="J27">
+        <v>1690</v>
+      </c>
+      <c r="K27" s="1">
+        <v>21</v>
+      </c>
+      <c r="L27" s="1">
+        <f>G27*60</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="1">
+        <f>H27*60</f>
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F6:M29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>1525</v>
+      </c>
+      <c r="J7">
+        <v>1560</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <f>G7*60</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <f>H7*60</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>1525</v>
+      </c>
+      <c r="J8">
+        <v>1560</v>
+      </c>
+      <c r="K8" s="1">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" ref="L8:M26" si="0">G8*60</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>1525</v>
+      </c>
+      <c r="J9">
+        <v>1560</v>
+      </c>
+      <c r="K9" s="1">
+        <v>3</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>1525</v>
+      </c>
+      <c r="J10">
+        <v>1560</v>
+      </c>
+      <c r="K10" s="1">
+        <v>4</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>1525</v>
+      </c>
+      <c r="J11">
+        <v>1560</v>
+      </c>
+      <c r="K11" s="1">
+        <v>5</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>1525</v>
+      </c>
+      <c r="J12">
+        <v>1560</v>
+      </c>
+      <c r="K12" s="1">
+        <v>6</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>1525</v>
+      </c>
+      <c r="J13">
+        <v>1560</v>
+      </c>
+      <c r="K13" s="1">
+        <v>7</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>1525</v>
+      </c>
+      <c r="J14">
+        <v>1560</v>
+      </c>
+      <c r="K14" s="1">
+        <v>8</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>1525</v>
+      </c>
+      <c r="J15">
+        <v>1560</v>
+      </c>
+      <c r="K15" s="1">
+        <v>9</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>1525</v>
+      </c>
+      <c r="J16">
+        <v>1560</v>
+      </c>
+      <c r="K16" s="1">
+        <v>10</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>1525</v>
+      </c>
+      <c r="J17">
+        <v>1560</v>
+      </c>
+      <c r="K17" s="1">
+        <v>11</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>1525</v>
+      </c>
+      <c r="J18">
+        <v>1560</v>
+      </c>
+      <c r="K18" s="1">
+        <v>12</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>1525</v>
+      </c>
+      <c r="J19">
+        <v>1560</v>
+      </c>
+      <c r="K19" s="1">
+        <v>13</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>1525</v>
+      </c>
+      <c r="J20">
+        <v>1560</v>
+      </c>
+      <c r="K20" s="1">
+        <v>14</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>1525</v>
+      </c>
+      <c r="J21">
+        <v>1560</v>
+      </c>
+      <c r="K21" s="1">
+        <v>15</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>1525</v>
+      </c>
+      <c r="J22">
+        <v>1560</v>
+      </c>
+      <c r="K22" s="1">
+        <v>16</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>1525</v>
+      </c>
+      <c r="J23">
+        <v>1560</v>
+      </c>
+      <c r="K23" s="1">
+        <v>17</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="24" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>1525</v>
+      </c>
+      <c r="J24">
+        <v>1560</v>
+      </c>
+      <c r="K24" s="1">
+        <v>18</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>1525</v>
+      </c>
+      <c r="J25">
+        <v>1560</v>
+      </c>
+      <c r="K25" s="1">
+        <v>19</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>1525</v>
+      </c>
+      <c r="J26">
+        <v>1560</v>
+      </c>
+      <c r="K26" s="1">
+        <v>20</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>1525</v>
+      </c>
+      <c r="J27">
+        <v>1560</v>
+      </c>
+      <c r="K27" s="1">
+        <v>21</v>
+      </c>
+      <c r="L27" s="1">
+        <f>G27*60</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="1">
+        <f>H27*60</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>90</v>
+      </c>
+      <c r="I28">
+        <v>1525</v>
+      </c>
+      <c r="J28">
+        <v>1560</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L28" s="3">
+        <f>G28*60</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="3">
+        <f>H28*60</f>
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="29" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>5</v>
+      </c>
+      <c r="I29">
+        <v>1525</v>
+      </c>
+      <c r="J29">
+        <v>1560</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="3">
+        <f>G29*60</f>
+        <v>120</v>
+      </c>
+      <c r="M29" s="3">
+        <f>H29*60</f>
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F6:M29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>1815</v>
+      </c>
+      <c r="J7">
+        <v>1875</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <f>G7*60</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <f>H7*60</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>1815</v>
+      </c>
+      <c r="J8">
+        <v>1875</v>
+      </c>
+      <c r="K8" s="1">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" ref="L8:M26" si="0">G8*60</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>1815</v>
+      </c>
+      <c r="J9">
+        <v>1875</v>
+      </c>
+      <c r="K9" s="1">
+        <v>3</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>1815</v>
+      </c>
+      <c r="J10">
+        <v>1875</v>
+      </c>
+      <c r="K10" s="1">
+        <v>4</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>1815</v>
+      </c>
+      <c r="J11">
+        <v>1875</v>
+      </c>
+      <c r="K11" s="1">
+        <v>5</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>1815</v>
+      </c>
+      <c r="J12">
+        <v>1875</v>
+      </c>
+      <c r="K12" s="1">
+        <v>6</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>1815</v>
+      </c>
+      <c r="J13">
+        <v>1875</v>
+      </c>
+      <c r="K13" s="1">
+        <v>7</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>1815</v>
+      </c>
+      <c r="J14">
+        <v>1875</v>
+      </c>
+      <c r="K14" s="1">
+        <v>8</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>1815</v>
+      </c>
+      <c r="J15">
+        <v>1875</v>
+      </c>
+      <c r="K15" s="1">
+        <v>9</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>1815</v>
+      </c>
+      <c r="J16">
+        <v>1875</v>
+      </c>
+      <c r="K16" s="1">
+        <v>10</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>1815</v>
+      </c>
+      <c r="J17">
+        <v>1875</v>
+      </c>
+      <c r="K17" s="1">
+        <v>11</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>1815</v>
+      </c>
+      <c r="J18">
+        <v>1875</v>
+      </c>
+      <c r="K18" s="1">
+        <v>12</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>1815</v>
+      </c>
+      <c r="J19">
+        <v>1875</v>
+      </c>
+      <c r="K19" s="1">
+        <v>13</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>1815</v>
+      </c>
+      <c r="J20">
+        <v>1875</v>
+      </c>
+      <c r="K20" s="1">
+        <v>14</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>1815</v>
+      </c>
+      <c r="J21">
+        <v>1875</v>
+      </c>
+      <c r="K21" s="1">
+        <v>15</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>1815</v>
+      </c>
+      <c r="J22">
+        <v>1875</v>
+      </c>
+      <c r="K22" s="1">
+        <v>16</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>1815</v>
+      </c>
+      <c r="J23">
+        <v>1875</v>
+      </c>
+      <c r="K23" s="1">
+        <v>17</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="24" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>1815</v>
+      </c>
+      <c r="J24">
+        <v>1875</v>
+      </c>
+      <c r="K24" s="1">
+        <v>18</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>1815</v>
+      </c>
+      <c r="J25">
+        <v>1875</v>
+      </c>
+      <c r="K25" s="1">
+        <v>19</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>1815</v>
+      </c>
+      <c r="J26">
+        <v>1875</v>
+      </c>
+      <c r="K26" s="1">
+        <v>20</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>1815</v>
+      </c>
+      <c r="J27">
+        <v>1875</v>
+      </c>
+      <c r="K27" s="1">
+        <v>21</v>
+      </c>
+      <c r="L27" s="1">
+        <f>G27*60</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="1">
+        <f>H27*60</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28">
+        <v>1815</v>
+      </c>
+      <c r="J28">
+        <v>1875</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L28" s="3">
+        <f>G28*60</f>
+        <v>120</v>
+      </c>
+      <c r="M28" s="3">
+        <f>H28*60</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="29" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F29" s="2"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>